<commit_message>
fix the bug of function SendMsg
</commit_message>
<xml_diff>
--- a/Bin/resource/excel/Scene.xlsx
+++ b/Bin/resource/excel/Scene.xlsx
@@ -229,12 +229,22 @@
     <t>34.10933,1.165174,11.49214</t>
   </si>
   <si>
-    <t>../resource/res/Scene/1.xml</t>
+    <t>../resource/res/map/1.xml</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t>../resource</t>
+      <t>../resource/res/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>map</t>
     </r>
     <r>
       <rPr>
@@ -243,7 +253,23 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>/</t>
+      <t>/2.xml</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>../resource/res/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>map</t>
     </r>
     <r>
       <rPr>
@@ -252,7 +278,23 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>res</t>
+      <t>/3.xml</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>../resource/res/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>map</t>
     </r>
     <r>
       <rPr>
@@ -261,13 +303,23 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>/Scene/2.xml</t>
+      <t>/4.xml</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <r>
-      <t>../resource</t>
+      <t>../resource/res/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>map</t>
     </r>
     <r>
       <rPr>
@@ -276,7 +328,23 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>/</t>
+      <t>/5.xml</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>../resource/res/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>map</t>
     </r>
     <r>
       <rPr>
@@ -285,115 +353,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>res</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/Scene/3.xml</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>../resource</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>res</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/Scene/4.xml</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>../resource</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>res</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/Scene/5.xml</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>../resource</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>res</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color indexed="8"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>/Scene/6.xml</t>
+      <t>/6.xml</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -402,7 +362,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -412,6 +372,13 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -437,8 +404,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -790,7 +760,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1260,7 +1230,7 @@
       <c r="E10">
         <v>200</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="1" t="s">
         <v>62</v>
       </c>
       <c r="G10" t="s">
@@ -1310,7 +1280,7 @@
       <c r="E11">
         <v>200</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>63</v>
       </c>
       <c r="G11" t="s">
@@ -1360,7 +1330,7 @@
       <c r="E12">
         <v>200</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="1" t="s">
         <v>64</v>
       </c>
       <c r="G12" t="s">
@@ -1410,7 +1380,7 @@
       <c r="E13">
         <v>200</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="1" t="s">
         <v>65</v>
       </c>
       <c r="G13" t="s">
@@ -1460,7 +1430,7 @@
       <c r="E14">
         <v>200</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G14" t="s">

</xml_diff>